<commit_message>
changed the creation of the AO-1 report for the new initial template
</commit_message>
<xml_diff>
--- a/reports/example_advance_report.xlsx
+++ b/reports/example_advance_report.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист_1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Лист_1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -377,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -690,6 +690,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1292,7 +1304,7 @@
         </is>
       </c>
       <c r="R9" s="37" t="n">
-        <v>13194</v>
+        <v>129023</v>
       </c>
       <c r="S9" s="92" t="n"/>
       <c r="T9" s="92" t="n"/>
@@ -1304,7 +1316,7 @@
         </is>
       </c>
       <c r="X9" s="18" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Y9" s="36" t="inlineStr">
         <is>
@@ -1361,7 +1373,7 @@
       <c r="I13" s="91" t="n"/>
       <c r="J13" s="42" t="inlineStr">
         <is>
-          <t>13.02.2025</t>
+          <t>15.02.2025</t>
         </is>
       </c>
       <c r="K13" s="90" t="n"/>
@@ -1396,7 +1408,7 @@
     <row r="15" ht="10.9" customFormat="1" customHeight="1" s="2">
       <c r="O15" s="45" t="inlineStr">
         <is>
-          <t>13 февраля 2025 г.</t>
+          <t>15 февраля 2025 г.</t>
         </is>
       </c>
       <c r="P15" s="92" t="n"/>
@@ -1436,7 +1448,7 @@
       </c>
       <c r="H19" s="48" t="inlineStr">
         <is>
-          <t>Региональный проект</t>
+          <t>Региональное подразделение</t>
         </is>
       </c>
       <c r="I19" s="92" t="n"/>
@@ -1477,7 +1489,7 @@
       </c>
       <c r="F21" s="50" t="inlineStr">
         <is>
-          <t>Петров Андрей Владимирович</t>
+          <t>Бойко А.А.</t>
         </is>
       </c>
       <c r="G21" s="92" t="n"/>
@@ -1821,7 +1833,7 @@
       <c r="H33" s="90" t="n"/>
       <c r="I33" s="91" t="n"/>
       <c r="J33" s="60" t="n">
-        <v>13194.2</v>
+        <v>129023.2</v>
       </c>
       <c r="K33" s="90" t="n"/>
       <c r="L33" s="91" t="n"/>
@@ -1932,7 +1944,7 @@
       </c>
       <c r="J39" s="106" t="inlineStr">
         <is>
-          <t>Тринадцать тысяч сто девяносто четыре рублей 20 копеек (13194 руб. 20 коп.)</t>
+          <t>Сто двадцать девять тысяч двадцать три рублей 19 копеек (129023 руб. 19 коп.)</t>
         </is>
       </c>
     </row>
@@ -2145,7 +2157,7 @@
       </c>
       <c r="I55" s="109" t="inlineStr">
         <is>
-          <t>Петров Андрей Владимирович</t>
+          <t>Бойко А.А.</t>
         </is>
       </c>
       <c r="P55" s="100" t="inlineStr">
@@ -2163,7 +2175,7 @@
       </c>
       <c r="D56" s="106" t="inlineStr">
         <is>
-          <t>13 февраля 2025 г.</t>
+          <t>15 февраля 2025 г.</t>
         </is>
       </c>
       <c r="H56" s="110" t="inlineStr">
@@ -2173,7 +2185,7 @@
       </c>
       <c r="K56" s="111" t="inlineStr">
         <is>
-          <t>Тринадцать тысяч сто девяносто четыре рублей 20 копеек (13194 руб. 20 коп.)</t>
+          <t>Сто двадцать девять тысяч двадцать три рублей 19 копеек (129023 руб. 19 коп.)</t>
         </is>
       </c>
       <c r="X56" s="105" t="inlineStr">
@@ -2439,25 +2451,25 @@
         <v>1</v>
       </c>
       <c r="C66" s="115" t="n"/>
-      <c r="D66" s="115" t="inlineStr">
-        <is>
-          <t>01.08.2023</t>
+      <c r="D66" s="116" t="inlineStr">
+        <is>
+          <t>01.02.2025</t>
         </is>
       </c>
       <c r="E66" s="115" t="n"/>
-      <c r="F66" s="115" t="n">
-        <v>1</v>
+      <c r="F66" s="117" t="n">
+        <v>1579</v>
       </c>
       <c r="G66" s="115" t="n"/>
-      <c r="H66" s="115" t="inlineStr">
-        <is>
-          <t>представительские - мероприятие</t>
+      <c r="H66" s="118" t="inlineStr">
+        <is>
+          <t>Кассовый чек Представительские расходы</t>
         </is>
       </c>
       <c r="I66" s="115" t="n"/>
       <c r="J66" s="115" t="n"/>
       <c r="K66" s="115" t="n"/>
-      <c r="L66" s="114" t="n">
+      <c r="L66" s="119" t="n">
         <v>5000.2</v>
       </c>
       <c r="M66" s="115" t="n"/>
@@ -2465,7 +2477,7 @@
       <c r="O66" s="115" t="n"/>
       <c r="P66" s="115" t="n"/>
       <c r="Q66" s="115" t="n"/>
-      <c r="R66" s="114" t="n">
+      <c r="R66" s="119" t="n">
         <v>5000.2</v>
       </c>
       <c r="S66" s="115" t="n"/>
@@ -2481,25 +2493,25 @@
         <v>2</v>
       </c>
       <c r="C67" s="115" t="n"/>
-      <c r="D67" s="115" t="inlineStr">
-        <is>
-          <t>01.08.2023</t>
+      <c r="D67" s="116" t="inlineStr">
+        <is>
+          <t>02.02.2025</t>
         </is>
       </c>
       <c r="E67" s="115" t="n"/>
-      <c r="F67" s="115" t="n">
-        <v>2</v>
+      <c r="F67" s="117" t="n">
+        <v>23</v>
       </c>
       <c r="G67" s="115" t="n"/>
-      <c r="H67" s="115" t="inlineStr">
-        <is>
-          <t>представительские - мероприятие</t>
+      <c r="H67" s="118" t="inlineStr">
+        <is>
+          <t>Кассовый чек Представительские расходы</t>
         </is>
       </c>
       <c r="I67" s="115" t="n"/>
       <c r="J67" s="115" t="n"/>
       <c r="K67" s="115" t="n"/>
-      <c r="L67" s="114" t="n">
+      <c r="L67" s="119" t="n">
         <v>789</v>
       </c>
       <c r="M67" s="115" t="n"/>
@@ -2507,7 +2519,7 @@
       <c r="O67" s="115" t="n"/>
       <c r="P67" s="115" t="n"/>
       <c r="Q67" s="115" t="n"/>
-      <c r="R67" s="114" t="n">
+      <c r="R67" s="119" t="n">
         <v>789</v>
       </c>
       <c r="S67" s="115" t="n"/>
@@ -2523,34 +2535,34 @@
         <v>3</v>
       </c>
       <c r="C68" s="115" t="n"/>
-      <c r="D68" s="115" t="inlineStr">
-        <is>
-          <t>02.08.2023</t>
+      <c r="D68" s="116" t="inlineStr">
+        <is>
+          <t>03.02.2025</t>
         </is>
       </c>
       <c r="E68" s="115" t="n"/>
-      <c r="F68" s="115" t="n">
-        <v>3</v>
+      <c r="F68" s="117" t="n">
+        <v>43</v>
       </c>
       <c r="G68" s="115" t="n"/>
-      <c r="H68" s="115" t="inlineStr">
-        <is>
-          <t>канцелярия</t>
+      <c r="H68" s="118" t="inlineStr">
+        <is>
+          <t>Чек ККТ</t>
         </is>
       </c>
       <c r="I68" s="115" t="n"/>
       <c r="J68" s="115" t="n"/>
       <c r="K68" s="115" t="n"/>
-      <c r="L68" s="114" t="n">
-        <v>12</v>
+      <c r="L68" s="119" t="n">
+        <v>300</v>
       </c>
       <c r="M68" s="115" t="n"/>
       <c r="N68" s="115" t="n"/>
       <c r="O68" s="115" t="n"/>
       <c r="P68" s="115" t="n"/>
       <c r="Q68" s="115" t="n"/>
-      <c r="R68" s="114" t="n">
-        <v>12</v>
+      <c r="R68" s="119" t="n">
+        <v>300</v>
       </c>
       <c r="S68" s="115" t="n"/>
       <c r="T68" s="115" t="n"/>
@@ -2565,34 +2577,34 @@
         <v>4</v>
       </c>
       <c r="C69" s="115" t="n"/>
-      <c r="D69" s="115" t="inlineStr">
-        <is>
-          <t>02.08.2023</t>
+      <c r="D69" s="116" t="inlineStr">
+        <is>
+          <t>05.02.2025</t>
         </is>
       </c>
       <c r="E69" s="115" t="n"/>
-      <c r="F69" s="115" t="n">
-        <v>4</v>
+      <c r="F69" s="117" t="n">
+        <v>7678678</v>
       </c>
       <c r="G69" s="115" t="n"/>
-      <c r="H69" s="115" t="inlineStr">
-        <is>
-          <t>гсм</t>
+      <c r="H69" s="118" t="inlineStr">
+        <is>
+          <t>Кассовый чек ГСМ</t>
         </is>
       </c>
       <c r="I69" s="115" t="n"/>
       <c r="J69" s="115" t="n"/>
       <c r="K69" s="115" t="n"/>
-      <c r="L69" s="114" t="n">
-        <v>12</v>
+      <c r="L69" s="119" t="n">
+        <v>4000</v>
       </c>
       <c r="M69" s="115" t="n"/>
       <c r="N69" s="115" t="n"/>
       <c r="O69" s="115" t="n"/>
       <c r="P69" s="115" t="n"/>
       <c r="Q69" s="115" t="n"/>
-      <c r="R69" s="114" t="n">
-        <v>12</v>
+      <c r="R69" s="119" t="n">
+        <v>4000</v>
       </c>
       <c r="S69" s="115" t="n"/>
       <c r="T69" s="115" t="n"/>
@@ -2607,34 +2619,34 @@
         <v>5</v>
       </c>
       <c r="C70" s="115" t="n"/>
-      <c r="D70" s="115" t="inlineStr">
-        <is>
-          <t>02.08.2023</t>
+      <c r="D70" s="116" t="inlineStr">
+        <is>
+          <t>08.02.2025</t>
         </is>
       </c>
       <c r="E70" s="115" t="n"/>
-      <c r="F70" s="115" t="n">
-        <v>5</v>
+      <c r="F70" s="117" t="n">
+        <v>456</v>
       </c>
       <c r="G70" s="115" t="n"/>
-      <c r="H70" s="115" t="inlineStr">
-        <is>
-          <t>представительские - мероприятие</t>
+      <c r="H70" s="118" t="inlineStr">
+        <is>
+          <t>Кассовый чек Представительские расходы</t>
         </is>
       </c>
       <c r="I70" s="115" t="n"/>
       <c r="J70" s="115" t="n"/>
       <c r="K70" s="115" t="n"/>
-      <c r="L70" s="114" t="n">
-        <v>12</v>
+      <c r="L70" s="119" t="n">
+        <v>15234</v>
       </c>
       <c r="M70" s="115" t="n"/>
       <c r="N70" s="115" t="n"/>
       <c r="O70" s="115" t="n"/>
       <c r="P70" s="115" t="n"/>
       <c r="Q70" s="115" t="n"/>
-      <c r="R70" s="114" t="n">
-        <v>12</v>
+      <c r="R70" s="119" t="n">
+        <v>15234</v>
       </c>
       <c r="S70" s="115" t="n"/>
       <c r="T70" s="115" t="n"/>
@@ -2649,34 +2661,36 @@
         <v>6</v>
       </c>
       <c r="C71" s="115" t="n"/>
-      <c r="D71" s="115" t="inlineStr">
-        <is>
-          <t>02.08.2023</t>
+      <c r="D71" s="116" t="inlineStr">
+        <is>
+          <t>10.02.2025</t>
         </is>
       </c>
       <c r="E71" s="115" t="n"/>
-      <c r="F71" s="115" t="n">
-        <v>6</v>
+      <c r="F71" s="117" t="inlineStr">
+        <is>
+          <t>456-Ю</t>
+        </is>
       </c>
       <c r="G71" s="115" t="n"/>
-      <c r="H71" s="115" t="inlineStr">
-        <is>
-          <t>представительские - мероприятие</t>
+      <c r="H71" s="118" t="inlineStr">
+        <is>
+          <t>Кассовый чек Представительские расходы</t>
         </is>
       </c>
       <c r="I71" s="115" t="n"/>
       <c r="J71" s="115" t="n"/>
       <c r="K71" s="115" t="n"/>
-      <c r="L71" s="114" t="n">
-        <v>12</v>
+      <c r="L71" s="119" t="n">
+        <v>17000</v>
       </c>
       <c r="M71" s="115" t="n"/>
       <c r="N71" s="115" t="n"/>
       <c r="O71" s="115" t="n"/>
       <c r="P71" s="115" t="n"/>
       <c r="Q71" s="115" t="n"/>
-      <c r="R71" s="114" t="n">
-        <v>12</v>
+      <c r="R71" s="119" t="n">
+        <v>17000</v>
       </c>
       <c r="S71" s="115" t="n"/>
       <c r="T71" s="115" t="n"/>
@@ -2691,19 +2705,25 @@
         <v>7</v>
       </c>
       <c r="C72" s="115" t="n"/>
-      <c r="D72" s="115" t="n"/>
+      <c r="D72" s="116" t="inlineStr">
+        <is>
+          <t>12.02.2025</t>
+        </is>
+      </c>
       <c r="E72" s="115" t="n"/>
-      <c r="F72" s="115" t="n"/>
+      <c r="F72" s="117" t="n">
+        <v>954322</v>
+      </c>
       <c r="G72" s="115" t="n"/>
-      <c r="H72" s="115" t="inlineStr">
-        <is>
-          <t>суточные</t>
+      <c r="H72" s="118" t="inlineStr">
+        <is>
+          <t>Кассовый чек Суточные</t>
         </is>
       </c>
       <c r="I72" s="115" t="n"/>
       <c r="J72" s="115" t="n"/>
       <c r="K72" s="115" t="n"/>
-      <c r="L72" s="114" t="n">
+      <c r="L72" s="119" t="n">
         <v>7225</v>
       </c>
       <c r="M72" s="115" t="n"/>
@@ -2711,7 +2731,7 @@
       <c r="O72" s="115" t="n"/>
       <c r="P72" s="115" t="n"/>
       <c r="Q72" s="115" t="n"/>
-      <c r="R72" s="114" t="n">
+      <c r="R72" s="119" t="n">
         <v>7225</v>
       </c>
       <c r="S72" s="115" t="n"/>
@@ -2727,34 +2747,34 @@
         <v>8</v>
       </c>
       <c r="C73" s="115" t="n"/>
-      <c r="D73" s="115" t="inlineStr">
-        <is>
-          <t>02.08.2023</t>
+      <c r="D73" s="116" t="inlineStr">
+        <is>
+          <t>13.02.2025</t>
         </is>
       </c>
       <c r="E73" s="115" t="n"/>
-      <c r="F73" s="115" t="n">
-        <v>8</v>
+      <c r="F73" s="117" t="n">
+        <v>34563</v>
       </c>
       <c r="G73" s="115" t="n"/>
-      <c r="H73" s="115" t="inlineStr">
-        <is>
-          <t>представительские - мероприятие</t>
+      <c r="H73" s="118" t="inlineStr">
+        <is>
+          <t>Чек ККТ</t>
         </is>
       </c>
       <c r="I73" s="115" t="n"/>
       <c r="J73" s="115" t="n"/>
       <c r="K73" s="115" t="n"/>
-      <c r="L73" s="114" t="n">
-        <v>12</v>
+      <c r="L73" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="M73" s="115" t="n"/>
       <c r="N73" s="115" t="n"/>
       <c r="O73" s="115" t="n"/>
       <c r="P73" s="115" t="n"/>
       <c r="Q73" s="115" t="n"/>
-      <c r="R73" s="114" t="n">
-        <v>12</v>
+      <c r="R73" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="S73" s="115" t="n"/>
       <c r="T73" s="115" t="n"/>
@@ -2769,34 +2789,34 @@
         <v>9</v>
       </c>
       <c r="C74" s="115" t="n"/>
-      <c r="D74" s="115" t="inlineStr">
-        <is>
-          <t>02.08.2023</t>
+      <c r="D74" s="116" t="inlineStr">
+        <is>
+          <t>14.02.2025</t>
         </is>
       </c>
       <c r="E74" s="115" t="n"/>
-      <c r="F74" s="115" t="n">
-        <v>9</v>
+      <c r="F74" s="117" t="n">
+        <v>34563</v>
       </c>
       <c r="G74" s="115" t="n"/>
-      <c r="H74" s="115" t="inlineStr">
-        <is>
-          <t>представительские - мероприятие</t>
+      <c r="H74" s="118" t="inlineStr">
+        <is>
+          <t>Кассовый чек Представительские расходы</t>
         </is>
       </c>
       <c r="I74" s="115" t="n"/>
       <c r="J74" s="115" t="n"/>
       <c r="K74" s="115" t="n"/>
-      <c r="L74" s="114" t="n">
-        <v>12</v>
+      <c r="L74" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="M74" s="115" t="n"/>
       <c r="N74" s="115" t="n"/>
       <c r="O74" s="115" t="n"/>
       <c r="P74" s="115" t="n"/>
       <c r="Q74" s="115" t="n"/>
-      <c r="R74" s="114" t="n">
-        <v>12</v>
+      <c r="R74" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="S74" s="115" t="n"/>
       <c r="T74" s="115" t="n"/>
@@ -2811,34 +2831,34 @@
         <v>10</v>
       </c>
       <c r="C75" s="115" t="n"/>
-      <c r="D75" s="115" t="inlineStr">
-        <is>
-          <t>02.08.2023</t>
+      <c r="D75" s="116" t="inlineStr">
+        <is>
+          <t>15.02.2025</t>
         </is>
       </c>
       <c r="E75" s="115" t="n"/>
-      <c r="F75" s="115" t="n">
-        <v>10</v>
+      <c r="F75" s="117" t="n">
+        <v>34563</v>
       </c>
       <c r="G75" s="115" t="n"/>
-      <c r="H75" s="115" t="inlineStr">
-        <is>
-          <t>представительские - мероприятие</t>
+      <c r="H75" s="118" t="inlineStr">
+        <is>
+          <t>Кассовый чек Представительские расходы</t>
         </is>
       </c>
       <c r="I75" s="115" t="n"/>
       <c r="J75" s="115" t="n"/>
       <c r="K75" s="115" t="n"/>
-      <c r="L75" s="114" t="n">
-        <v>12</v>
+      <c r="L75" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="M75" s="115" t="n"/>
       <c r="N75" s="115" t="n"/>
       <c r="O75" s="115" t="n"/>
       <c r="P75" s="115" t="n"/>
       <c r="Q75" s="115" t="n"/>
-      <c r="R75" s="114" t="n">
-        <v>12</v>
+      <c r="R75" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="S75" s="115" t="n"/>
       <c r="T75" s="115" t="n"/>
@@ -2853,34 +2873,34 @@
         <v>11</v>
       </c>
       <c r="C76" s="115" t="n"/>
-      <c r="D76" s="115" t="inlineStr">
-        <is>
-          <t>02.08.2023</t>
+      <c r="D76" s="116" t="inlineStr">
+        <is>
+          <t>16.02.2025</t>
         </is>
       </c>
       <c r="E76" s="115" t="n"/>
-      <c r="F76" s="115" t="n">
-        <v>11</v>
+      <c r="F76" s="117" t="n">
+        <v>34563</v>
       </c>
       <c r="G76" s="115" t="n"/>
-      <c r="H76" s="115" t="inlineStr">
-        <is>
-          <t>представительские - мероприятие</t>
+      <c r="H76" s="118" t="inlineStr">
+        <is>
+          <t>Кассовый чек Представительские расходы</t>
         </is>
       </c>
       <c r="I76" s="115" t="n"/>
       <c r="J76" s="115" t="n"/>
       <c r="K76" s="115" t="n"/>
-      <c r="L76" s="114" t="n">
-        <v>12</v>
+      <c r="L76" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="M76" s="115" t="n"/>
       <c r="N76" s="115" t="n"/>
       <c r="O76" s="115" t="n"/>
       <c r="P76" s="115" t="n"/>
       <c r="Q76" s="115" t="n"/>
-      <c r="R76" s="114" t="n">
-        <v>12</v>
+      <c r="R76" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="S76" s="115" t="n"/>
       <c r="T76" s="115" t="n"/>
@@ -2895,34 +2915,34 @@
         <v>12</v>
       </c>
       <c r="C77" s="115" t="n"/>
-      <c r="D77" s="115" t="inlineStr">
-        <is>
-          <t>02.08.2023</t>
+      <c r="D77" s="116" t="inlineStr">
+        <is>
+          <t>17.02.2025</t>
         </is>
       </c>
       <c r="E77" s="115" t="n"/>
-      <c r="F77" s="115" t="n">
-        <v>12</v>
+      <c r="F77" s="117" t="n">
+        <v>34563</v>
       </c>
       <c r="G77" s="115" t="n"/>
-      <c r="H77" s="115" t="inlineStr">
-        <is>
-          <t>представительские - мероприятие</t>
+      <c r="H77" s="118" t="inlineStr">
+        <is>
+          <t>Кассовый чек Представительские расходы</t>
         </is>
       </c>
       <c r="I77" s="115" t="n"/>
       <c r="J77" s="115" t="n"/>
       <c r="K77" s="115" t="n"/>
-      <c r="L77" s="114" t="n">
-        <v>12</v>
+      <c r="L77" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="M77" s="115" t="n"/>
       <c r="N77" s="115" t="n"/>
       <c r="O77" s="115" t="n"/>
       <c r="P77" s="115" t="n"/>
       <c r="Q77" s="115" t="n"/>
-      <c r="R77" s="114" t="n">
-        <v>12</v>
+      <c r="R77" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="S77" s="115" t="n"/>
       <c r="T77" s="115" t="n"/>
@@ -2937,34 +2957,34 @@
         <v>13</v>
       </c>
       <c r="C78" s="115" t="n"/>
-      <c r="D78" s="115" t="inlineStr">
-        <is>
-          <t>02.08.2023</t>
+      <c r="D78" s="116" t="inlineStr">
+        <is>
+          <t>18.02.2025</t>
         </is>
       </c>
       <c r="E78" s="115" t="n"/>
-      <c r="F78" s="115" t="n">
-        <v>13</v>
+      <c r="F78" s="117" t="n">
+        <v>34563</v>
       </c>
       <c r="G78" s="115" t="n"/>
-      <c r="H78" s="115" t="inlineStr">
-        <is>
-          <t>представительские - мероприятие</t>
+      <c r="H78" s="118" t="inlineStr">
+        <is>
+          <t>Кассовый чек Представительские расходы</t>
         </is>
       </c>
       <c r="I78" s="115" t="n"/>
       <c r="J78" s="115" t="n"/>
       <c r="K78" s="115" t="n"/>
-      <c r="L78" s="114" t="n">
-        <v>12</v>
+      <c r="L78" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="M78" s="115" t="n"/>
       <c r="N78" s="115" t="n"/>
       <c r="O78" s="115" t="n"/>
       <c r="P78" s="115" t="n"/>
       <c r="Q78" s="115" t="n"/>
-      <c r="R78" s="114" t="n">
-        <v>12</v>
+      <c r="R78" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="S78" s="115" t="n"/>
       <c r="T78" s="115" t="n"/>
@@ -2979,34 +2999,34 @@
         <v>14</v>
       </c>
       <c r="C79" s="115" t="n"/>
-      <c r="D79" s="115" t="inlineStr">
-        <is>
-          <t>02.08.2023</t>
+      <c r="D79" s="116" t="inlineStr">
+        <is>
+          <t>19.02.2025</t>
         </is>
       </c>
       <c r="E79" s="115" t="n"/>
-      <c r="F79" s="115" t="n">
-        <v>14</v>
+      <c r="F79" s="117" t="n">
+        <v>34563</v>
       </c>
       <c r="G79" s="115" t="n"/>
-      <c r="H79" s="115" t="inlineStr">
-        <is>
-          <t>представительские - мероприятие</t>
+      <c r="H79" s="118" t="inlineStr">
+        <is>
+          <t>Кассовый чек Представительские расходы</t>
         </is>
       </c>
       <c r="I79" s="115" t="n"/>
       <c r="J79" s="115" t="n"/>
       <c r="K79" s="115" t="n"/>
-      <c r="L79" s="114" t="n">
-        <v>12</v>
+      <c r="L79" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="M79" s="115" t="n"/>
       <c r="N79" s="115" t="n"/>
       <c r="O79" s="115" t="n"/>
       <c r="P79" s="115" t="n"/>
       <c r="Q79" s="115" t="n"/>
-      <c r="R79" s="114" t="n">
-        <v>12</v>
+      <c r="R79" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="S79" s="115" t="n"/>
       <c r="T79" s="115" t="n"/>
@@ -3021,34 +3041,34 @@
         <v>15</v>
       </c>
       <c r="C80" s="115" t="n"/>
-      <c r="D80" s="115" t="inlineStr">
-        <is>
-          <t>02.08.2023</t>
+      <c r="D80" s="116" t="inlineStr">
+        <is>
+          <t>20.02.2025</t>
         </is>
       </c>
       <c r="E80" s="115" t="n"/>
-      <c r="F80" s="115" t="n">
-        <v>15</v>
+      <c r="F80" s="117" t="n">
+        <v>34563</v>
       </c>
       <c r="G80" s="115" t="n"/>
-      <c r="H80" s="115" t="inlineStr">
-        <is>
-          <t>представительские - мероприятие</t>
+      <c r="H80" s="118" t="inlineStr">
+        <is>
+          <t>Кассовый чек Представительские расходы</t>
         </is>
       </c>
       <c r="I80" s="115" t="n"/>
       <c r="J80" s="115" t="n"/>
       <c r="K80" s="115" t="n"/>
-      <c r="L80" s="114" t="n">
-        <v>12</v>
+      <c r="L80" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="M80" s="115" t="n"/>
       <c r="N80" s="115" t="n"/>
       <c r="O80" s="115" t="n"/>
       <c r="P80" s="115" t="n"/>
       <c r="Q80" s="115" t="n"/>
-      <c r="R80" s="114" t="n">
-        <v>12</v>
+      <c r="R80" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="S80" s="115" t="n"/>
       <c r="T80" s="115" t="n"/>
@@ -3063,34 +3083,34 @@
         <v>16</v>
       </c>
       <c r="C81" s="115" t="n"/>
-      <c r="D81" s="115" t="inlineStr">
-        <is>
-          <t>02.08.2023</t>
+      <c r="D81" s="116" t="inlineStr">
+        <is>
+          <t>21.02.2025</t>
         </is>
       </c>
       <c r="E81" s="115" t="n"/>
-      <c r="F81" s="115" t="n">
-        <v>16</v>
+      <c r="F81" s="117" t="n">
+        <v>34563</v>
       </c>
       <c r="G81" s="115" t="n"/>
-      <c r="H81" s="115" t="inlineStr">
-        <is>
-          <t>представительские - мероприятие</t>
+      <c r="H81" s="118" t="inlineStr">
+        <is>
+          <t>Кассовый чек Представительские расходы</t>
         </is>
       </c>
       <c r="I81" s="115" t="n"/>
       <c r="J81" s="115" t="n"/>
       <c r="K81" s="115" t="n"/>
-      <c r="L81" s="114" t="n">
-        <v>12</v>
+      <c r="L81" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="M81" s="115" t="n"/>
       <c r="N81" s="115" t="n"/>
       <c r="O81" s="115" t="n"/>
       <c r="P81" s="115" t="n"/>
       <c r="Q81" s="115" t="n"/>
-      <c r="R81" s="114" t="n">
-        <v>12</v>
+      <c r="R81" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="S81" s="115" t="n"/>
       <c r="T81" s="115" t="n"/>
@@ -3105,34 +3125,34 @@
         <v>17</v>
       </c>
       <c r="C82" s="115" t="n"/>
-      <c r="D82" s="115" t="inlineStr">
-        <is>
-          <t>02.08.2023</t>
+      <c r="D82" s="116" t="inlineStr">
+        <is>
+          <t>22.02.2025</t>
         </is>
       </c>
       <c r="E82" s="115" t="n"/>
-      <c r="F82" s="115" t="n">
-        <v>17</v>
+      <c r="F82" s="117" t="n">
+        <v>34563</v>
       </c>
       <c r="G82" s="115" t="n"/>
-      <c r="H82" s="115" t="inlineStr">
-        <is>
-          <t>представительские - мероприятие</t>
+      <c r="H82" s="118" t="inlineStr">
+        <is>
+          <t>Кассовый чек Представительские расходы</t>
         </is>
       </c>
       <c r="I82" s="115" t="n"/>
       <c r="J82" s="115" t="n"/>
       <c r="K82" s="115" t="n"/>
-      <c r="L82" s="114" t="n">
-        <v>12</v>
+      <c r="L82" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="M82" s="115" t="n"/>
       <c r="N82" s="115" t="n"/>
       <c r="O82" s="115" t="n"/>
       <c r="P82" s="115" t="n"/>
       <c r="Q82" s="115" t="n"/>
-      <c r="R82" s="114" t="n">
-        <v>12</v>
+      <c r="R82" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="S82" s="115" t="n"/>
       <c r="T82" s="115" t="n"/>
@@ -3147,34 +3167,34 @@
         <v>18</v>
       </c>
       <c r="C83" s="115" t="n"/>
-      <c r="D83" s="115" t="inlineStr">
-        <is>
-          <t>02.08.2023</t>
+      <c r="D83" s="116" t="inlineStr">
+        <is>
+          <t>23.02.2025</t>
         </is>
       </c>
       <c r="E83" s="115" t="n"/>
-      <c r="F83" s="115" t="n">
-        <v>18</v>
+      <c r="F83" s="117" t="n">
+        <v>34563</v>
       </c>
       <c r="G83" s="115" t="n"/>
-      <c r="H83" s="115" t="inlineStr">
-        <is>
-          <t>представительские - мероприятие</t>
+      <c r="H83" s="118" t="inlineStr">
+        <is>
+          <t>Кассовый чек Представительские расходы</t>
         </is>
       </c>
       <c r="I83" s="115" t="n"/>
       <c r="J83" s="115" t="n"/>
       <c r="K83" s="115" t="n"/>
-      <c r="L83" s="114" t="n">
-        <v>12</v>
+      <c r="L83" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="M83" s="115" t="n"/>
       <c r="N83" s="115" t="n"/>
       <c r="O83" s="115" t="n"/>
       <c r="P83" s="115" t="n"/>
       <c r="Q83" s="115" t="n"/>
-      <c r="R83" s="114" t="n">
-        <v>12</v>
+      <c r="R83" s="119" t="n">
+        <v>7225</v>
       </c>
       <c r="S83" s="115" t="n"/>
       <c r="T83" s="115" t="n"/>
@@ -3196,22 +3216,22 @@
           <t>Итого</t>
         </is>
       </c>
-      <c r="L84" s="116">
+      <c r="L84" s="120">
         <f>SUM(L66:L83)</f>
         <v/>
       </c>
       <c r="M84" s="115" t="n"/>
       <c r="N84" s="115" t="n"/>
-      <c r="O84" s="116" t="n"/>
+      <c r="O84" s="120" t="n"/>
       <c r="P84" s="115" t="n"/>
       <c r="Q84" s="115" t="n"/>
-      <c r="R84" s="116">
+      <c r="R84" s="120">
         <f>SUM(R66:R83)</f>
         <v/>
       </c>
       <c r="S84" s="115" t="n"/>
       <c r="T84" s="115" t="n"/>
-      <c r="U84" s="116" t="n"/>
+      <c r="U84" s="120" t="n"/>
       <c r="V84" s="115" t="n"/>
       <c r="W84" s="115" t="n"/>
       <c r="X84" s="88" t="n"/>
@@ -3250,30 +3270,30 @@
           <t>Подотчетное лицо</t>
         </is>
       </c>
-      <c r="F86" s="117" t="n"/>
-      <c r="G86" s="118" t="n"/>
-      <c r="H86" s="118" t="n"/>
-      <c r="I86" s="118" t="n"/>
-      <c r="J86" s="118" t="n"/>
-      <c r="K86" s="118" t="n"/>
-      <c r="L86" s="118" t="n"/>
+      <c r="F86" s="121" t="n"/>
+      <c r="G86" s="122" t="n"/>
+      <c r="H86" s="122" t="n"/>
+      <c r="I86" s="122" t="n"/>
+      <c r="J86" s="122" t="n"/>
+      <c r="K86" s="122" t="n"/>
+      <c r="L86" s="122" t="n"/>
       <c r="M86" s="88" t="n"/>
-      <c r="N86" s="117" t="inlineStr">
-        <is>
-          <t>Петров Андрей Владимирович</t>
-        </is>
-      </c>
-      <c r="O86" s="118" t="n"/>
-      <c r="P86" s="118" t="n"/>
-      <c r="Q86" s="118" t="n"/>
-      <c r="R86" s="118" t="n"/>
-      <c r="S86" s="118" t="n"/>
-      <c r="T86" s="118" t="n"/>
-      <c r="U86" s="118" t="n"/>
-      <c r="V86" s="118" t="n"/>
-      <c r="W86" s="118" t="n"/>
-      <c r="X86" s="118" t="n"/>
-      <c r="Y86" s="118" t="n"/>
+      <c r="N86" s="121" t="inlineStr">
+        <is>
+          <t>Бойко А.А.</t>
+        </is>
+      </c>
+      <c r="O86" s="122" t="n"/>
+      <c r="P86" s="122" t="n"/>
+      <c r="Q86" s="122" t="n"/>
+      <c r="R86" s="122" t="n"/>
+      <c r="S86" s="122" t="n"/>
+      <c r="T86" s="122" t="n"/>
+      <c r="U86" s="122" t="n"/>
+      <c r="V86" s="122" t="n"/>
+      <c r="W86" s="122" t="n"/>
+      <c r="X86" s="122" t="n"/>
+      <c r="Y86" s="122" t="n"/>
       <c r="AB86" s="20" t="n"/>
     </row>
     <row r="87" ht="11" customHeight="1" s="24">
@@ -3281,13 +3301,13 @@
       <c r="C87" s="86" t="n"/>
       <c r="D87" s="88" t="n"/>
       <c r="E87" s="88" t="n"/>
-      <c r="F87" s="119" t="inlineStr">
+      <c r="F87" s="123" t="inlineStr">
         <is>
           <t>подпись</t>
         </is>
       </c>
       <c r="M87" s="88" t="n"/>
-      <c r="N87" s="119" t="inlineStr">
+      <c r="N87" s="123" t="inlineStr">
         <is>
           <t>расшифровка подписи</t>
         </is>
@@ -3353,30 +3373,30 @@
           <t>Руководитель</t>
         </is>
       </c>
-      <c r="F90" s="118" t="n"/>
-      <c r="G90" s="118" t="n"/>
-      <c r="H90" s="118" t="n"/>
-      <c r="I90" s="118" t="n"/>
-      <c r="J90" s="118" t="n"/>
-      <c r="K90" s="118" t="n"/>
-      <c r="L90" s="118" t="n"/>
+      <c r="F90" s="122" t="n"/>
+      <c r="G90" s="122" t="n"/>
+      <c r="H90" s="122" t="n"/>
+      <c r="I90" s="122" t="n"/>
+      <c r="J90" s="122" t="n"/>
+      <c r="K90" s="122" t="n"/>
+      <c r="L90" s="122" t="n"/>
       <c r="M90" s="22" t="n"/>
-      <c r="N90" s="120" t="inlineStr">
-        <is>
-          <t>Петров Андрей Владимирович</t>
-        </is>
-      </c>
-      <c r="O90" s="118" t="n"/>
-      <c r="P90" s="118" t="n"/>
-      <c r="Q90" s="118" t="n"/>
-      <c r="R90" s="118" t="n"/>
-      <c r="S90" s="118" t="n"/>
-      <c r="T90" s="118" t="n"/>
-      <c r="U90" s="118" t="n"/>
-      <c r="V90" s="118" t="n"/>
-      <c r="W90" s="118" t="n"/>
-      <c r="X90" s="118" t="n"/>
-      <c r="Y90" s="118" t="n"/>
+      <c r="N90" s="124" t="inlineStr">
+        <is>
+          <t>Бойко А.А.</t>
+        </is>
+      </c>
+      <c r="O90" s="122" t="n"/>
+      <c r="P90" s="122" t="n"/>
+      <c r="Q90" s="122" t="n"/>
+      <c r="R90" s="122" t="n"/>
+      <c r="S90" s="122" t="n"/>
+      <c r="T90" s="122" t="n"/>
+      <c r="U90" s="122" t="n"/>
+      <c r="V90" s="122" t="n"/>
+      <c r="W90" s="122" t="n"/>
+      <c r="X90" s="122" t="n"/>
+      <c r="Y90" s="122" t="n"/>
     </row>
     <row r="91">
       <c r="B91" s="21" t="n"/>

</xml_diff>